<commit_message>
Made an intro scene, figured out text objects
</commit_message>
<xml_diff>
--- a/ScrumArtifacts/EECS448GameProject_ProductBacklog.xlsx
+++ b/ScrumArtifacts/EECS448GameProject_ProductBacklog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21960" windowHeight="16840" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="65">
   <si>
     <t>EECS 448 Project 4: Product Backlog</t>
   </si>
@@ -205,6 +205,15 @@
   </si>
   <si>
     <t>Very Heavy =</t>
+  </si>
+  <si>
+    <t>Moderate</t>
+  </si>
+  <si>
+    <t>Very Heavy</t>
+  </si>
+  <si>
+    <t>Heavy</t>
   </si>
 </sst>
 </file>
@@ -311,17 +320,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="35">
@@ -691,7 +700,7 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -703,34 +712,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="30">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="3" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="4" t="s">
         <v>58</v>
       </c>
       <c r="F3" t="s">
@@ -747,7 +756,7 @@
       <c r="C4" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="4" t="s">
         <v>59</v>
       </c>
       <c r="F4" t="s">
@@ -761,7 +770,10 @@
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="C5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>60</v>
       </c>
       <c r="F5" t="s">
@@ -775,7 +787,10 @@
       <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="C6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>61</v>
       </c>
       <c r="F6" t="s">
@@ -789,6 +804,9 @@
       <c r="B7" t="s">
         <v>18</v>
       </c>
+      <c r="C7" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
@@ -797,6 +815,9 @@
       <c r="B8" t="s">
         <v>20</v>
       </c>
+      <c r="C8" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
@@ -805,6 +826,9 @@
       <c r="B9" t="s">
         <v>22</v>
       </c>
+      <c r="C9" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
@@ -813,6 +837,9 @@
       <c r="B10" t="s">
         <v>24</v>
       </c>
+      <c r="C10" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
@@ -821,6 +848,9 @@
       <c r="B11" t="s">
         <v>26</v>
       </c>
+      <c r="C11" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
@@ -829,9 +859,12 @@
       <c r="B12" t="s">
         <v>28</v>
       </c>
+      <c r="C12" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -842,145 +875,193 @@
       <c r="B15" t="s">
         <v>16</v>
       </c>
+      <c r="C15" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>32</v>
       </c>
       <c r="B17" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>35</v>
       </c>
       <c r="B18" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="C18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>34</v>
       </c>
       <c r="B19" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="C19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>32</v>
       </c>
       <c r="B21" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="C21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>35</v>
       </c>
       <c r="B22" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="C22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>43</v>
       </c>
       <c r="B23" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="C23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>34</v>
       </c>
       <c r="B24" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="C24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>45</v>
       </c>
       <c r="B25" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="C25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>32</v>
       </c>
       <c r="B27" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
+      <c r="C27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>35</v>
       </c>
       <c r="B28" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
+      <c r="C28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>43</v>
       </c>
       <c r="B29" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
+      <c r="C29" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
         <v>34</v>
       </c>
       <c r="B30" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
+      <c r="C30" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
         <v>45</v>
       </c>
       <c r="B31" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="5" t="s">
+      <c r="C31" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
         <v>10</v>
       </c>
       <c r="B34" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="35" spans="1:2">
+      <c r="C34" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35" t="s">
         <v>29</v>
       </c>
       <c r="B35" t="s">
         <v>30</v>
+      </c>
+      <c r="C35" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>